<commit_message>
bug fixed: file repository
</commit_message>
<xml_diff>
--- a/d_classchart.xlsx
+++ b/d_classchart.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f1a78db8ae5a5339/桌面/code/Python/ClassCompare_teach/ClassCompare/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f1a78db8ae5a5339/桌面/code/Python/ClassCompare/ClassCompare/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_EA687DB7836F74CFEB3B98154BAC56386E97F6C2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B8D24647-8E9D-45E6-8E5B-DD248A75FC45}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_EA68B3AFC36AFCCFEB3B98154B7F8E3C5D0BF727" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{69D899F4-4161-437E-B698-E90B0EF80F60}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -444,7 +444,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12:F19"/>
+      <selection activeCell="C12" sqref="C12:D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>

</xml_diff>